<commit_message>
Add UBER Q4 2025 recurring cycle: earnings analysis, model update, morning note, Q1 2026 preview
Post-Q4 2025 earnings analysis with actual results vs consensus, thesis impact assessment,
and updated target price ($100 -> $109). Model update with target price bridge, assumptions
revision, updated projections, and DCF revision. Morning note with price action and catalyst
calendar. Q1 2026 earnings preview with scenarios and positioning recommendation.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/coverage/UBER/04-financial-model/3-statements.xlsx
+++ b/coverage/UBER/04-financial-model/3-statements.xlsx
@@ -138,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -179,7 +179,6 @@
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -546,7 +545,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,13 +561,12 @@
     <col width="13" customWidth="1" min="6" max="6"/>
     <col width="13" customWidth="1" min="7" max="7"/>
     <col width="13" customWidth="1" min="8" max="8"/>
-    <col width="13" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Key Assumptions — UBER (Uber Technologies)</t>
+          <t>Key Assumptions � UBER (Uber Technologies) [UPDATED POST Q4-2025]</t>
         </is>
       </c>
     </row>
@@ -604,14 +602,9 @@
           <t>2028E</t>
         </is>
       </c>
-      <c r="H3" s="4" t="inlineStr">
+      <c r="H3" s="2" t="inlineStr">
         <is>
           <t>2029E</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>2030E</t>
         </is>
       </c>
     </row>
@@ -622,28 +615,25 @@
         </is>
       </c>
       <c r="B4" s="6" t="n">
-        <v>0.169</v>
+        <v>0.143</v>
       </c>
       <c r="C4" s="6" t="n">
-        <v>0.18</v>
+        <v>0.177</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>0.183</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>0.17</v>
+        <v>0.178</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>0.15</v>
+        <v>0.155</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>0.13</v>
+        <v>0.136</v>
       </c>
       <c r="H4" s="7" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="I4" s="7" t="n">
-        <v>0.1</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="5">
@@ -653,28 +643,25 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>0.627</v>
+        <v>0.632</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>0.625</v>
       </c>
       <c r="D5" s="6" t="n">
+        <v>0.618</v>
+      </c>
+      <c r="E5" s="7" t="n">
         <v>0.615</v>
       </c>
-      <c r="E5" s="7" t="n">
-        <v>0.61</v>
-      </c>
       <c r="F5" s="7" t="n">
+        <v>0.608</v>
+      </c>
+      <c r="G5" s="7" t="n">
         <v>0.6</v>
       </c>
-      <c r="G5" s="7" t="n">
-        <v>0.59</v>
-      </c>
       <c r="H5" s="7" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="I5" s="7" t="n">
-        <v>0.575</v>
+        <v>0.592</v>
       </c>
     </row>
     <row r="6">
@@ -684,28 +671,25 @@
         </is>
       </c>
       <c r="B6" s="6" t="n">
-        <v>0.137</v>
+        <v>0.125</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>0.12</v>
+        <v>0.115</v>
       </c>
       <c r="D6" s="6" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="E6" s="7" t="n">
         <v>0.11</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="F6" s="7" t="n">
         <v>0.105</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="G6" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="H6" s="7" t="n">
         <v>0.095</v>
-      </c>
-      <c r="H6" s="7" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="I6" s="7" t="n">
-        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -715,13 +699,13 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>0.15</v>
+        <v>0.126</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>0.131</v>
+        <v>0.12</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>0.12</v>
+        <v>0.117</v>
       </c>
       <c r="E7" s="7" t="n">
         <v>0.115</v>
@@ -735,9 +719,6 @@
       <c r="H7" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="I7" s="7" t="n">
-        <v>0.098</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
@@ -746,13 +727,13 @@
         </is>
       </c>
       <c r="B8" s="6" t="n">
-        <v>0.076</v>
+        <v>0.06</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>0.06</v>
+        <v>0.055</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>0.055</v>
+        <v>0.053</v>
       </c>
       <c r="E8" s="7" t="n">
         <v>0.052</v>
@@ -764,10 +745,7 @@
         <v>0.048</v>
       </c>
       <c r="H8" s="7" t="n">
-        <v>0.046</v>
-      </c>
-      <c r="I8" s="7" t="n">
-        <v>0.044</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="9">
@@ -777,28 +755,25 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>0.035</v>
+        <v>0.02</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>0.028</v>
+        <v>0.02</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>0.027</v>
+        <v>0.02</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>0.026</v>
+        <v>0.02</v>
       </c>
       <c r="H9" s="7" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="I9" s="7" t="n">
-        <v>0.025</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="10">
@@ -808,16 +783,16 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="E10" s="7" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="F10" s="7" t="n">
         <v>0.21</v>
@@ -828,9 +803,6 @@
       <c r="H10" s="7" t="n">
         <v>0.21</v>
       </c>
-      <c r="I10" s="7" t="n">
-        <v>0.21</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="inlineStr"/>
@@ -842,28 +814,25 @@
         </is>
       </c>
       <c r="B12" s="6" t="n">
-        <v>0.035</v>
+        <v>0.02</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>0.035</v>
+        <v>0.022</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>0.033</v>
+        <v>0.022</v>
       </c>
       <c r="E12" s="7" t="n">
-        <v>0.032</v>
+        <v>0.022</v>
       </c>
       <c r="F12" s="7" t="n">
-        <v>0.03</v>
+        <v>0.023</v>
       </c>
       <c r="G12" s="7" t="n">
-        <v>0.028</v>
+        <v>0.023</v>
       </c>
       <c r="H12" s="7" t="n">
-        <v>0.026</v>
-      </c>
-      <c r="I12" s="7" t="n">
-        <v>0.025</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="13">
@@ -873,28 +842,25 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="9" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D13" s="9" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E13" s="10" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F13" s="10" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G13" s="10" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H13" s="10" t="n">
-        <v>21</v>
-      </c>
-      <c r="I13" s="10" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
@@ -904,28 +870,25 @@
         </is>
       </c>
       <c r="B14" s="9" t="n">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C14" s="9" t="n">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D14" s="9" t="n">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="E14" s="10" t="n">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F14" s="10" t="n">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="G14" s="10" t="n">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="H14" s="10" t="n">
-        <v>42</v>
-      </c>
-      <c r="I14" s="10" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
@@ -935,28 +898,25 @@
         </is>
       </c>
       <c r="B15" s="6" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>0.058</v>
+        <v>0.078</v>
       </c>
       <c r="D15" s="6" t="n">
-        <v>0.055</v>
+        <v>0.075</v>
       </c>
       <c r="E15" s="7" t="n">
-        <v>0.053</v>
+        <v>0.073</v>
       </c>
       <c r="F15" s="7" t="n">
-        <v>0.051</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="G15" s="7" t="n">
-        <v>0.05</v>
+        <v>0.068</v>
       </c>
       <c r="H15" s="7" t="n">
-        <v>0.048</v>
-      </c>
-      <c r="I15" s="7" t="n">
-        <v>0.047</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="16">
@@ -972,25 +932,22 @@
         <v>0.05</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>0.052</v>
+        <v>0.05</v>
       </c>
       <c r="D17" s="6" t="n">
-        <v>0.053</v>
+        <v>0.048</v>
       </c>
       <c r="E17" s="7" t="n">
-        <v>0.053</v>
+        <v>0.048</v>
       </c>
       <c r="F17" s="7" t="n">
-        <v>0.053</v>
+        <v>0.046</v>
       </c>
       <c r="G17" s="7" t="n">
-        <v>0.052</v>
+        <v>0.044</v>
       </c>
       <c r="H17" s="7" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="I17" s="7" t="n">
-        <v>0.048</v>
+        <v>0.042</v>
       </c>
     </row>
     <row r="18">
@@ -1000,28 +957,25 @@
         </is>
       </c>
       <c r="B18" s="11" t="n">
-        <v>2050</v>
+        <v>2052</v>
       </c>
       <c r="C18" s="11" t="n">
-        <v>2070</v>
+        <v>2068</v>
       </c>
       <c r="D18" s="11" t="n">
         <v>2084</v>
       </c>
       <c r="E18" s="12" t="n">
-        <v>2060</v>
+        <v>2042</v>
       </c>
       <c r="F18" s="12" t="n">
-        <v>2040</v>
+        <v>2000</v>
       </c>
       <c r="G18" s="12" t="n">
-        <v>2020</v>
+        <v>1960</v>
       </c>
       <c r="H18" s="12" t="n">
-        <v>2000</v>
-      </c>
-      <c r="I18" s="12" t="n">
-        <v>1980</v>
+        <v>1920</v>
       </c>
     </row>
   </sheetData>
@@ -1036,7 +990,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1052,13 +1006,12 @@
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="14" customWidth="1" min="7" max="7"/>
     <col width="14" customWidth="1" min="8" max="8"/>
-    <col width="14" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Income Statement — UBER ($M)</t>
+          <t>Income Statement � UBER ($M) [UPDATED POST Q4-2025]</t>
         </is>
       </c>
     </row>
@@ -1099,11 +1052,6 @@
           <t>2029E</t>
         </is>
       </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>2030E</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
@@ -1115,7 +1063,7 @@
         <v>37281</v>
       </c>
       <c r="C4" s="14" t="n">
-        <v>43978</v>
+        <v>43953</v>
       </c>
       <c r="D4" s="14" t="n">
         <v>52020</v>
@@ -1132,12 +1080,8 @@
         <f>F4*(1+Assumptions!G4)</f>
         <v/>
       </c>
-      <c r="H4" s="15">
+      <c r="H4">
         <f>G4*(1+Assumptions!H4)</f>
-        <v/>
-      </c>
-      <c r="I4">
-        <f>H4*(1+Assumptions!I4)</f>
         <v/>
       </c>
     </row>
@@ -1148,7 +1092,7 @@
         </is>
       </c>
       <c r="B5" s="16" t="n">
-        <v>0.169</v>
+        <v>0.143</v>
       </c>
       <c r="C5" s="16">
         <f>(C4-B4)/B4</f>
@@ -1170,12 +1114,8 @@
         <f>Assumptions!G4</f>
         <v/>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="16">
         <f>Assumptions!H4</f>
-        <v/>
-      </c>
-      <c r="I5" s="16">
-        <f>Assumptions!I4</f>
         <v/>
       </c>
     </row>
@@ -1186,13 +1126,13 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>23384</v>
+        <v>23567</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>27486</v>
+        <v>27471</v>
       </c>
       <c r="D6" s="14" t="n">
-        <v>31990</v>
+        <v>32149</v>
       </c>
       <c r="E6" s="15">
         <f>E4*Assumptions!E5</f>
@@ -1206,12 +1146,8 @@
         <f>G4*Assumptions!G5</f>
         <v/>
       </c>
-      <c r="H6" s="15">
+      <c r="H6">
         <f>H4*Assumptions!H5</f>
-        <v/>
-      </c>
-      <c r="I6">
-        <f>I4*Assumptions!I5</f>
         <v/>
       </c>
     </row>
@@ -1245,12 +1181,8 @@
         <f>G4-G6</f>
         <v/>
       </c>
-      <c r="H7" s="20">
+      <c r="H7">
         <f>H4-H6</f>
-        <v/>
-      </c>
-      <c r="I7">
-        <f>I4-I6</f>
         <v/>
       </c>
     </row>
@@ -1284,12 +1216,8 @@
         <f>G7/G4</f>
         <v/>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <f>H7/H4</f>
-        <v/>
-      </c>
-      <c r="I8" s="16">
-        <f>I7/I4</f>
         <v/>
       </c>
     </row>
@@ -1298,7 +1226,6 @@
       <c r="E9" s="21" t="n"/>
       <c r="F9" s="21" t="n"/>
       <c r="G9" s="21" t="n"/>
-      <c r="H9" s="21" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="8" t="inlineStr">
@@ -1307,13 +1234,13 @@
         </is>
       </c>
       <c r="B10" s="14" t="n">
-        <v>5111</v>
+        <v>4661</v>
       </c>
       <c r="C10" s="14" t="n">
-        <v>5277</v>
+        <v>5055</v>
       </c>
       <c r="D10" s="14" t="n">
-        <v>5722</v>
+        <v>5618</v>
       </c>
       <c r="E10" s="15">
         <f>E4*Assumptions!E6</f>
@@ -1327,12 +1254,8 @@
         <f>G4*Assumptions!G6</f>
         <v/>
       </c>
-      <c r="H10" s="15">
+      <c r="H10">
         <f>H4*Assumptions!H6</f>
-        <v/>
-      </c>
-      <c r="I10">
-        <f>I4*Assumptions!I6</f>
         <v/>
       </c>
     </row>
@@ -1343,13 +1266,13 @@
         </is>
       </c>
       <c r="B11" s="14" t="n">
-        <v>5593</v>
+        <v>4698</v>
       </c>
       <c r="C11" s="14" t="n">
-        <v>5780</v>
+        <v>5274</v>
       </c>
       <c r="D11" s="14" t="n">
-        <v>6242</v>
+        <v>6086</v>
       </c>
       <c r="E11" s="15">
         <f>E4*Assumptions!E7</f>
@@ -1363,12 +1286,8 @@
         <f>G4*Assumptions!G7</f>
         <v/>
       </c>
-      <c r="H11" s="15">
+      <c r="H11">
         <f>H4*Assumptions!H7</f>
-        <v/>
-      </c>
-      <c r="I11">
-        <f>I4*Assumptions!I7</f>
         <v/>
       </c>
     </row>
@@ -1379,13 +1298,13 @@
         </is>
       </c>
       <c r="B12" s="14" t="n">
-        <v>2833</v>
+        <v>2238</v>
       </c>
       <c r="C12" s="14" t="n">
-        <v>2643</v>
+        <v>2418</v>
       </c>
       <c r="D12" s="14" t="n">
-        <v>2861</v>
+        <v>2757</v>
       </c>
       <c r="E12" s="15">
         <f>E4*Assumptions!E8</f>
@@ -1399,12 +1318,8 @@
         <f>G4*Assumptions!G8</f>
         <v/>
       </c>
-      <c r="H12" s="15">
+      <c r="H12">
         <f>H4*Assumptions!H8</f>
-        <v/>
-      </c>
-      <c r="I12">
-        <f>I4*Assumptions!I8</f>
         <v/>
       </c>
     </row>
@@ -1438,12 +1353,8 @@
         <f>G10+G11+G12</f>
         <v/>
       </c>
-      <c r="H13" s="24">
+      <c r="H13">
         <f>H10+H11+H12</f>
-        <v/>
-      </c>
-      <c r="I13">
-        <f>I10+I11+I12</f>
         <v/>
       </c>
     </row>
@@ -1452,7 +1363,6 @@
       <c r="E14" s="21" t="n"/>
       <c r="F14" s="21" t="n"/>
       <c r="G14" s="21" t="n"/>
-      <c r="H14" s="21" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="18" t="inlineStr">
@@ -1484,12 +1394,8 @@
         <f>G7-G13</f>
         <v/>
       </c>
-      <c r="H15" s="20">
+      <c r="H15">
         <f>H7-H13</f>
-        <v/>
-      </c>
-      <c r="I15">
-        <f>I7-I13</f>
         <v/>
       </c>
     </row>
@@ -1523,12 +1429,8 @@
         <f>G15/G4</f>
         <v/>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="16">
         <f>H15/H4</f>
-        <v/>
-      </c>
-      <c r="I16" s="16">
-        <f>I15/I4</f>
         <v/>
       </c>
     </row>
@@ -1537,7 +1439,6 @@
       <c r="E17" s="21" t="n"/>
       <c r="F17" s="21" t="n"/>
       <c r="G17" s="21" t="n"/>
-      <c r="H17" s="21" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="8" t="inlineStr">
@@ -1546,32 +1447,28 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>633</v>
+        <v>465</v>
       </c>
       <c r="C18" s="14" t="n">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="D18" s="14" t="n">
-        <v>380</v>
+        <v>456</v>
       </c>
       <c r="E18" s="25">
-        <f>'Balance Sheet'!E20*Assumptions!E17</f>
+        <f>'Balance Sheet'!E14*Assumptions!E17</f>
         <v/>
       </c>
       <c r="F18" s="25">
-        <f>'Balance Sheet'!F20*Assumptions!F17</f>
+        <f>'Balance Sheet'!F14*Assumptions!F17</f>
         <v/>
       </c>
       <c r="G18" s="25">
-        <f>'Balance Sheet'!G20*Assumptions!G17</f>
-        <v/>
-      </c>
-      <c r="H18" s="25">
-        <f>'Balance Sheet'!H20*Assumptions!H17</f>
-        <v/>
-      </c>
-      <c r="I18" s="26">
-        <f>'Balance Sheet'!I20*Assumptions!I17</f>
+        <f>'Balance Sheet'!G14*Assumptions!G17</f>
+        <v/>
+      </c>
+      <c r="H18" s="26">
+        <f>'Balance Sheet'!H14*Assumptions!H17</f>
         <v/>
       </c>
     </row>
@@ -1582,28 +1479,25 @@
         </is>
       </c>
       <c r="B19" s="14" t="n">
-        <v>-2676</v>
+        <v>-600</v>
       </c>
       <c r="C19" s="14" t="n">
-        <v>7146</v>
+        <v>1800</v>
       </c>
       <c r="D19" s="14" t="n">
-        <v>5238</v>
+        <v>900</v>
       </c>
       <c r="E19" s="27" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="F19" s="27" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="G19" s="27" t="n">
-        <v>300</v>
-      </c>
-      <c r="H19" s="27" t="n">
-        <v>300</v>
-      </c>
-      <c r="I19" s="28" t="n">
-        <v>300</v>
+        <v>500</v>
+      </c>
+      <c r="H19" s="28" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="20">
@@ -1636,12 +1530,8 @@
         <f>G15-G18+G19</f>
         <v/>
       </c>
-      <c r="H20" s="24">
+      <c r="H20">
         <f>H15-H18+H19</f>
-        <v/>
-      </c>
-      <c r="I20">
-        <f>I15-I18+I19</f>
         <v/>
       </c>
     </row>
@@ -1675,12 +1565,8 @@
         <f>G20*Assumptions!G10</f>
         <v/>
       </c>
-      <c r="H21" s="15">
+      <c r="H21">
         <f>H20*Assumptions!H10</f>
-        <v/>
-      </c>
-      <c r="I21">
-        <f>I20*Assumptions!I10</f>
         <v/>
       </c>
     </row>
@@ -1714,12 +1600,8 @@
         <f>IF(G20=0,0,G21/G20)</f>
         <v/>
       </c>
-      <c r="H22" s="17">
+      <c r="H22" s="16">
         <f>IF(H20=0,0,H21/H20)</f>
-        <v/>
-      </c>
-      <c r="I22" s="16">
-        <f>IF(I20=0,0,I21/I20)</f>
         <v/>
       </c>
     </row>
@@ -1753,12 +1635,8 @@
         <f>G20-G21</f>
         <v/>
       </c>
-      <c r="H23" s="20">
+      <c r="H23">
         <f>H20-H21</f>
-        <v/>
-      </c>
-      <c r="I23">
-        <f>I20-I21</f>
         <v/>
       </c>
     </row>
@@ -1792,12 +1670,8 @@
         <f>G23/G4</f>
         <v/>
       </c>
-      <c r="H24" s="17">
+      <c r="H24" s="16">
         <f>H23/H4</f>
-        <v/>
-      </c>
-      <c r="I24" s="16">
-        <f>I23/I4</f>
         <v/>
       </c>
     </row>
@@ -1806,7 +1680,6 @@
       <c r="E25" s="21" t="n"/>
       <c r="F25" s="21" t="n"/>
       <c r="G25" s="21" t="n"/>
-      <c r="H25" s="21" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="13" t="inlineStr">
@@ -1838,12 +1711,8 @@
         <f>G23/Assumptions!G18</f>
         <v/>
       </c>
-      <c r="H26" s="31">
+      <c r="H26" s="30">
         <f>H23/Assumptions!H18</f>
-        <v/>
-      </c>
-      <c r="I26" s="30">
-        <f>I23/Assumptions!I18</f>
         <v/>
       </c>
     </row>
@@ -1877,12 +1746,8 @@
         <f>G15+G4*Assumptions!G9</f>
         <v/>
       </c>
-      <c r="H27" s="24">
+      <c r="H27">
         <f>H15+H4*Assumptions!H9</f>
-        <v/>
-      </c>
-      <c r="I27">
-        <f>I15+I4*Assumptions!I9</f>
         <v/>
       </c>
     </row>
@@ -1916,12 +1781,8 @@
         <f>G27/G4</f>
         <v/>
       </c>
-      <c r="H28" s="17">
+      <c r="H28" s="16">
         <f>H27/H4</f>
-        <v/>
-      </c>
-      <c r="I28" s="16">
-        <f>I27/I4</f>
         <v/>
       </c>
     </row>
@@ -1937,7 +1798,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1953,13 +1814,12 @@
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="14" customWidth="1" min="7" max="7"/>
     <col width="14" customWidth="1" min="8" max="8"/>
-    <col width="14" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Balance Sheet — UBER ($M)</t>
+          <t>Balance Sheet � UBER ($M) [UPDATED POST Q4-2025]</t>
         </is>
       </c>
     </row>
@@ -2000,11 +1860,6 @@
           <t>2029E</t>
         </is>
       </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>2030E</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
@@ -2020,10 +1875,10 @@
         </is>
       </c>
       <c r="B5" s="14" t="n">
-        <v>4680</v>
+        <v>5088</v>
       </c>
       <c r="C5" s="14" t="n">
-        <v>5470</v>
+        <v>5700</v>
       </c>
       <c r="D5" s="14" t="n">
         <v>7000</v>
@@ -2040,12 +1895,8 @@
         <f>F5+'Cash Flow'!G19</f>
         <v/>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="26">
         <f>G5+'Cash Flow'!H19</f>
-        <v/>
-      </c>
-      <c r="I5" s="26">
-        <f>H5+'Cash Flow'!I19</f>
         <v/>
       </c>
     </row>
@@ -2056,13 +1907,13 @@
         </is>
       </c>
       <c r="B6" s="14" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
       <c r="C6" s="14" t="n">
-        <v>1700</v>
+        <v>1000</v>
       </c>
       <c r="D6" s="14" t="n">
-        <v>2000</v>
+        <v>1200</v>
       </c>
       <c r="E6" s="29">
         <f>D6*1.05</f>
@@ -2076,12 +1927,8 @@
         <f>F6*1.05</f>
         <v/>
       </c>
-      <c r="H6" s="29">
+      <c r="H6">
         <f>G6*1.05</f>
-        <v/>
-      </c>
-      <c r="I6">
-        <f>H6*1.05</f>
         <v/>
       </c>
     </row>
@@ -2092,13 +1939,13 @@
         </is>
       </c>
       <c r="B7" s="14" t="n">
-        <v>2560</v>
+        <v>2249</v>
       </c>
       <c r="C7" s="14" t="n">
-        <v>2890</v>
+        <v>2403</v>
       </c>
       <c r="D7" s="14" t="n">
-        <v>3280</v>
+        <v>2708</v>
       </c>
       <c r="E7" s="29">
         <f>'Income Statement'!E4*Assumptions!E13/365</f>
@@ -2112,12 +1959,8 @@
         <f>'Income Statement'!G4*Assumptions!G13/365</f>
         <v/>
       </c>
-      <c r="H7" s="29">
+      <c r="H7">
         <f>'Income Statement'!H4*Assumptions!H13/365</f>
-        <v/>
-      </c>
-      <c r="I7">
-        <f>'Income Statement'!I4*Assumptions!I13/365</f>
         <v/>
       </c>
     </row>
@@ -2131,10 +1974,10 @@
         <v>1800</v>
       </c>
       <c r="C8" s="14" t="n">
-        <v>2100</v>
+        <v>2000</v>
       </c>
       <c r="D8" s="14" t="n">
-        <v>2500</v>
+        <v>2300</v>
       </c>
       <c r="E8" s="29">
         <f>D8*1.05</f>
@@ -2148,12 +1991,8 @@
         <f>F8*1.05</f>
         <v/>
       </c>
-      <c r="H8" s="29">
+      <c r="H8">
         <f>G8*1.05</f>
-        <v/>
-      </c>
-      <c r="I8">
-        <f>H8*1.05</f>
         <v/>
       </c>
     </row>
@@ -2187,12 +2026,8 @@
         <f>SUM(G5:G8)</f>
         <v/>
       </c>
-      <c r="H9" s="33">
+      <c r="H9">
         <f>SUM(H5:H8)</f>
-        <v/>
-      </c>
-      <c r="I9">
-        <f>SUM(I5:I8)</f>
         <v/>
       </c>
     </row>
@@ -2206,13 +2041,13 @@
         </is>
       </c>
       <c r="B11" s="14" t="n">
-        <v>2370</v>
+        <v>2095</v>
       </c>
       <c r="C11" s="14" t="n">
-        <v>2550</v>
+        <v>2300</v>
       </c>
       <c r="D11" s="14" t="n">
-        <v>2700</v>
+        <v>2600</v>
       </c>
       <c r="E11" s="29">
         <f>D11+'Income Statement'!E4*Assumptions!E12-'Income Statement'!E4*Assumptions!E9</f>
@@ -2226,26 +2061,22 @@
         <f>F11+'Income Statement'!G4*Assumptions!G12-'Income Statement'!G4*Assumptions!G9</f>
         <v/>
       </c>
-      <c r="H11" s="29">
+      <c r="H11">
         <f>G11+'Income Statement'!H4*Assumptions!H12-'Income Statement'!H4*Assumptions!H9</f>
-        <v/>
-      </c>
-      <c r="I11">
-        <f>H11+'Income Statement'!I4*Assumptions!I12-'Income Statement'!I4*Assumptions!I9</f>
         <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="8" t="inlineStr">
         <is>
-          <t>Intangibles &amp; Goodwill</t>
+          <t>Goodwill</t>
         </is>
       </c>
       <c r="B12" s="14" t="n">
-        <v>16175</v>
+        <v>16100</v>
       </c>
       <c r="C12" s="14" t="n">
-        <v>16270</v>
+        <v>16300</v>
       </c>
       <c r="D12" s="14" t="n">
         <v>16300</v>
@@ -2262,12 +2093,8 @@
         <f>F12</f>
         <v/>
       </c>
-      <c r="H12" s="29">
+      <c r="H12">
         <f>G12</f>
-        <v/>
-      </c>
-      <c r="I12">
-        <f>H12</f>
         <v/>
       </c>
     </row>
@@ -2278,278 +2105,250 @@
         </is>
       </c>
       <c r="B13" s="14" t="n">
-        <v>12400</v>
+        <v>13800</v>
       </c>
       <c r="C13" s="14" t="n">
-        <v>14200</v>
+        <v>15000</v>
       </c>
       <c r="D13" s="14" t="n">
         <v>15000</v>
       </c>
       <c r="E13" s="29">
-        <f>D13*1.02</f>
+        <f>D13</f>
         <v/>
       </c>
       <c r="F13" s="29">
-        <f>E13*1.02</f>
+        <f>E13</f>
         <v/>
       </c>
       <c r="G13" s="29">
-        <f>F13*1.02</f>
-        <v/>
-      </c>
-      <c r="H13" s="29">
-        <f>G13*1.02</f>
-        <v/>
-      </c>
-      <c r="I13">
-        <f>H13*1.02</f>
+        <f>F13</f>
+        <v/>
+      </c>
+      <c r="H13">
+        <f>G13</f>
         <v/>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="inlineStr">
         <is>
+          <t>Long-Term Debt</t>
+        </is>
+      </c>
+      <c r="B14" s="14" t="n">
+        <v>9459</v>
+      </c>
+      <c r="C14" s="14" t="n">
+        <v>9500</v>
+      </c>
+      <c r="D14" s="14" t="n">
+        <v>9500</v>
+      </c>
+      <c r="E14" s="29">
+        <f>D14</f>
+        <v/>
+      </c>
+      <c r="F14" s="29">
+        <f>E14</f>
+        <v/>
+      </c>
+      <c r="G14" s="29">
+        <f>F14</f>
+        <v/>
+      </c>
+      <c r="H14">
+        <f>G14</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8" t="inlineStr">
+        <is>
           <t>Other Non-Current Assets</t>
         </is>
       </c>
-      <c r="B14" s="14" t="n">
-        <v>6715</v>
-      </c>
-      <c r="C14" s="14" t="n">
-        <v>7320</v>
-      </c>
-      <c r="D14" s="14" t="n">
-        <v>7520</v>
-      </c>
-      <c r="E14" s="29">
-        <f>D14*1.03</f>
-        <v/>
-      </c>
-      <c r="F14" s="29">
-        <f>E14*1.03</f>
-        <v/>
-      </c>
-      <c r="G14" s="29">
-        <f>F14*1.03</f>
-        <v/>
-      </c>
-      <c r="H14" s="29">
-        <f>G14*1.03</f>
-        <v/>
-      </c>
-      <c r="I14">
-        <f>H14*1.03</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="13" t="inlineStr">
+      <c r="B15" s="14" t="n">
+        <v>3200</v>
+      </c>
+      <c r="C15" s="14" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D15" s="14" t="n">
+        <v>3800</v>
+      </c>
+      <c r="E15" s="29">
+        <f>D15*1.03</f>
+        <v/>
+      </c>
+      <c r="F15" s="29">
+        <f>E15*1.03</f>
+        <v/>
+      </c>
+      <c r="G15" s="29">
+        <f>F15*1.03</f>
+        <v/>
+      </c>
+      <c r="H15">
+        <f>G15*1.03</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="13" t="inlineStr">
         <is>
           <t>Total Assets</t>
         </is>
       </c>
-      <c r="B15" s="33">
-        <f>B9+B11+B12+B13+B14</f>
-        <v/>
-      </c>
-      <c r="C15" s="33">
-        <f>C9+C11+C12+C13+C14</f>
-        <v/>
-      </c>
-      <c r="D15" s="33">
-        <f>D9+D11+D12+D13+D14</f>
-        <v/>
-      </c>
-      <c r="E15" s="33">
-        <f>E9+E11+E12+E13+E14</f>
-        <v/>
-      </c>
-      <c r="F15" s="33">
-        <f>F9+F11+F12+F13+F14</f>
-        <v/>
-      </c>
-      <c r="G15" s="33">
-        <f>G9+G11+G12+G13+G14</f>
-        <v/>
-      </c>
-      <c r="H15" s="33">
-        <f>H9+H11+H12+H13+H14</f>
-        <v/>
-      </c>
-      <c r="I15">
-        <f>I9+I11+I12+I13+I14</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="8" t="inlineStr"/>
+      <c r="B16" s="33">
+        <f>B9+B11+B12+B13+B14+B15</f>
+        <v/>
+      </c>
+      <c r="C16" s="33">
+        <f>C9+C11+C12+C13+C14+C15</f>
+        <v/>
+      </c>
+      <c r="D16" s="33">
+        <f>D9+D11+D12+D13+D14+D15</f>
+        <v/>
+      </c>
+      <c r="E16" s="33">
+        <f>E9+E11+E12+E13+E14+E15</f>
+        <v/>
+      </c>
+      <c r="F16" s="33">
+        <f>F9+F11+F12+F13+F14+F15</f>
+        <v/>
+      </c>
+      <c r="G16" s="33">
+        <f>G9+G11+G12+G13+G14+G15</f>
+        <v/>
+      </c>
+      <c r="H16">
+        <f>H9+H11+H12+H13+H14+H15</f>
+        <v/>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="13" t="inlineStr">
+      <c r="A17" s="8" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="13" t="inlineStr">
         <is>
           <t>LIABILITIES</t>
         </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="8" t="inlineStr">
-        <is>
-          <t>Accounts Payable</t>
-        </is>
-      </c>
-      <c r="B18" s="14" t="n">
-        <v>3200</v>
-      </c>
-      <c r="C18" s="14" t="n">
-        <v>3400</v>
-      </c>
-      <c r="D18" s="14" t="n">
-        <v>3600</v>
-      </c>
-      <c r="E18" s="29">
-        <f>'Income Statement'!E6*Assumptions!E14/365</f>
-        <v/>
-      </c>
-      <c r="F18" s="29">
-        <f>'Income Statement'!F6*Assumptions!F14/365</f>
-        <v/>
-      </c>
-      <c r="G18" s="29">
-        <f>'Income Statement'!G6*Assumptions!G14/365</f>
-        <v/>
-      </c>
-      <c r="H18" s="29">
-        <f>'Income Statement'!H6*Assumptions!H14/365</f>
-        <v/>
-      </c>
-      <c r="I18">
-        <f>'Income Statement'!I6*Assumptions!I14/365</f>
-        <v/>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="inlineStr">
         <is>
-          <t>Accrued Liabilities</t>
+          <t>Accounts Payable</t>
         </is>
       </c>
       <c r="B19" s="14" t="n">
-        <v>2237</v>
+        <v>1900</v>
       </c>
       <c r="C19" s="14" t="n">
-        <v>2550</v>
+        <v>2050</v>
       </c>
       <c r="D19" s="14" t="n">
-        <v>2860</v>
+        <v>2350</v>
       </c>
       <c r="E19" s="29">
-        <f>'Income Statement'!E4*Assumptions!E15</f>
+        <f>'Income Statement'!E6*Assumptions!E14/365</f>
         <v/>
       </c>
       <c r="F19" s="29">
-        <f>'Income Statement'!F4*Assumptions!F15</f>
+        <f>'Income Statement'!F6*Assumptions!F14/365</f>
         <v/>
       </c>
       <c r="G19" s="29">
-        <f>'Income Statement'!G4*Assumptions!G15</f>
-        <v/>
-      </c>
-      <c r="H19" s="29">
-        <f>'Income Statement'!H4*Assumptions!H15</f>
-        <v/>
-      </c>
-      <c r="I19">
-        <f>'Income Statement'!I4*Assumptions!I15</f>
+        <f>'Income Statement'!G6*Assumptions!G14/365</f>
+        <v/>
+      </c>
+      <c r="H19">
+        <f>'Income Statement'!H6*Assumptions!H14/365</f>
         <v/>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="inlineStr">
         <is>
-          <t>Long-Term Debt</t>
+          <t>Accrued Liabilities</t>
         </is>
       </c>
       <c r="B20" s="14" t="n">
-        <v>9400</v>
+        <v>2985</v>
       </c>
       <c r="C20" s="14" t="n">
-        <v>9800</v>
+        <v>3432</v>
       </c>
       <c r="D20" s="14" t="n">
-        <v>9500</v>
-      </c>
-      <c r="E20" s="14">
-        <f>D20*0.97</f>
-        <v/>
-      </c>
-      <c r="F20" s="14">
-        <f>E20*0.97</f>
-        <v/>
-      </c>
-      <c r="G20" s="14">
-        <f>F20*0.97</f>
-        <v/>
-      </c>
-      <c r="H20" s="14">
-        <f>G20*0.97</f>
-        <v/>
-      </c>
-      <c r="I20" s="28">
-        <f>H20*0.97</f>
+        <v>3903</v>
+      </c>
+      <c r="E20" s="29">
+        <f>'Income Statement'!E4*Assumptions!E15</f>
+        <v/>
+      </c>
+      <c r="F20" s="29">
+        <f>'Income Statement'!F4*Assumptions!F15</f>
+        <v/>
+      </c>
+      <c r="G20" s="29">
+        <f>'Income Statement'!G4*Assumptions!G15</f>
+        <v/>
+      </c>
+      <c r="H20">
+        <f>'Income Statement'!H4*Assumptions!H15</f>
         <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="inlineStr">
         <is>
-          <t>Operating Lease Liabilities</t>
+          <t>Short-Term Debt</t>
         </is>
       </c>
       <c r="B21" s="14" t="n">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="C21" s="14" t="n">
-        <v>1600</v>
+        <v>500</v>
       </c>
       <c r="D21" s="14" t="n">
-        <v>1700</v>
+        <v>500</v>
       </c>
       <c r="E21" s="29">
-        <f>D21*1.02</f>
+        <f>D21</f>
         <v/>
       </c>
       <c r="F21" s="29">
-        <f>E21*1.02</f>
+        <f>E21</f>
         <v/>
       </c>
       <c r="G21" s="29">
-        <f>F21*1.02</f>
-        <v/>
-      </c>
-      <c r="H21" s="29">
-        <f>G21*1.02</f>
-        <v/>
-      </c>
-      <c r="I21">
-        <f>H21*1.02</f>
+        <f>F21</f>
+        <v/>
+      </c>
+      <c r="H21">
+        <f>G21</f>
         <v/>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="8" t="inlineStr">
         <is>
-          <t>Other Liabilities</t>
+          <t>Other Current Liabilities</t>
         </is>
       </c>
       <c r="B22" s="14" t="n">
-        <v>4800</v>
+        <v>3000</v>
       </c>
       <c r="C22" s="14" t="n">
-        <v>5200</v>
+        <v>3200</v>
       </c>
       <c r="D22" s="14" t="n">
-        <v>5540</v>
+        <v>3500</v>
       </c>
       <c r="E22" s="29">
         <f>D22*1.03</f>
@@ -2563,51 +2362,43 @@
         <f>F22*1.03</f>
         <v/>
       </c>
-      <c r="H22" s="29">
+      <c r="H22">
         <f>G22*1.03</f>
-        <v/>
-      </c>
-      <c r="I22">
-        <f>H22*1.03</f>
         <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="13" t="inlineStr">
         <is>
-          <t>Total Liabilities</t>
+          <t>Total Current Liabilities</t>
         </is>
       </c>
       <c r="B23" s="33">
-        <f>B18+B19+B20+B21+B22</f>
+        <f>SUM(B19:B22)</f>
         <v/>
       </c>
       <c r="C23" s="33">
-        <f>C18+C19+C20+C21+C22</f>
+        <f>SUM(C19:C22)</f>
         <v/>
       </c>
       <c r="D23" s="33">
-        <f>D18+D19+D20+D21+D22</f>
+        <f>SUM(D19:D22)</f>
         <v/>
       </c>
       <c r="E23" s="33">
-        <f>E18+E19+E20+E21+E22</f>
+        <f>SUM(E19:E22)</f>
         <v/>
       </c>
       <c r="F23" s="33">
-        <f>F18+F19+F20+F21+F22</f>
+        <f>SUM(F19:F22)</f>
         <v/>
       </c>
       <c r="G23" s="33">
-        <f>G18+G19+G20+G21+G22</f>
-        <v/>
-      </c>
-      <c r="H23" s="33">
-        <f>H18+H19+H20+H21+H22</f>
-        <v/>
-      </c>
-      <c r="I23">
-        <f>I18+I19+I20+I21+I22</f>
+        <f>SUM(G19:G22)</f>
+        <v/>
+      </c>
+      <c r="H23">
+        <f>SUM(H19:H22)</f>
         <v/>
       </c>
     </row>
@@ -2615,201 +2406,283 @@
       <c r="A24" s="8" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="13" t="inlineStr">
-        <is>
-          <t>EQUITY</t>
-        </is>
+      <c r="A25" s="8" t="inlineStr">
+        <is>
+          <t>Long-Term Debt</t>
+        </is>
+      </c>
+      <c r="B25" s="14" t="n">
+        <v>9459</v>
+      </c>
+      <c r="C25" s="14" t="n">
+        <v>9500</v>
+      </c>
+      <c r="D25" s="14" t="n">
+        <v>9500</v>
+      </c>
+      <c r="E25" s="29">
+        <f>D25</f>
+        <v/>
+      </c>
+      <c r="F25" s="29">
+        <f>E25</f>
+        <v/>
+      </c>
+      <c r="G25" s="29">
+        <f>F25</f>
+        <v/>
+      </c>
+      <c r="H25">
+        <f>G25</f>
+        <v/>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="inlineStr">
         <is>
-          <t>Retained Earnings</t>
-        </is>
-      </c>
-      <c r="B26" s="34">
-        <f>B15-B23-B27</f>
-        <v/>
-      </c>
-      <c r="C26" s="34">
-        <f>C15-C23-C27</f>
-        <v/>
-      </c>
-      <c r="D26" s="34">
-        <f>D15-D23-D27</f>
-        <v/>
+          <t>Other Non-Current Liabilities</t>
+        </is>
+      </c>
+      <c r="B26" s="14" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C26" s="14" t="n">
+        <v>5200</v>
+      </c>
+      <c r="D26" s="14" t="n">
+        <v>5400</v>
       </c>
       <c r="E26" s="29">
-        <f>D26+'Income Statement'!E23</f>
+        <f>D26*1.02</f>
         <v/>
       </c>
       <c r="F26" s="29">
-        <f>E26+'Income Statement'!F23</f>
+        <f>E26*1.02</f>
         <v/>
       </c>
       <c r="G26" s="29">
-        <f>F26+'Income Statement'!G23</f>
-        <v/>
-      </c>
-      <c r="H26" s="29">
-        <f>G26+'Income Statement'!H23</f>
-        <v/>
-      </c>
-      <c r="I26">
-        <f>H26+'Income Statement'!I23</f>
+        <f>F26*1.02</f>
+        <v/>
+      </c>
+      <c r="H26">
+        <f>G26*1.02</f>
         <v/>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="8" t="inlineStr">
-        <is>
-          <t>Other Equity</t>
-        </is>
-      </c>
-      <c r="B27" s="14" t="n">
-        <v>20103</v>
-      </c>
-      <c r="C27" s="14" t="n">
-        <v>23290</v>
-      </c>
-      <c r="D27" s="14" t="n">
-        <v>28100</v>
-      </c>
-      <c r="E27" s="29">
-        <f>D27</f>
-        <v/>
-      </c>
-      <c r="F27" s="29">
-        <f>E27</f>
-        <v/>
-      </c>
-      <c r="G27" s="29">
-        <f>F27</f>
-        <v/>
-      </c>
-      <c r="H27" s="29">
-        <f>G27</f>
-        <v/>
-      </c>
-      <c r="I27">
-        <f>H27</f>
+      <c r="A27" s="13" t="inlineStr">
+        <is>
+          <t>Total Liabilities</t>
+        </is>
+      </c>
+      <c r="B27" s="33">
+        <f>B23+B25+B26</f>
+        <v/>
+      </c>
+      <c r="C27" s="33">
+        <f>C23+C25+C26</f>
+        <v/>
+      </c>
+      <c r="D27" s="33">
+        <f>D23+D25+D26</f>
+        <v/>
+      </c>
+      <c r="E27" s="33">
+        <f>E23+E25+E26</f>
+        <v/>
+      </c>
+      <c r="F27" s="33">
+        <f>F23+F25+F26</f>
+        <v/>
+      </c>
+      <c r="G27" s="33">
+        <f>G23+G25+G26</f>
+        <v/>
+      </c>
+      <c r="H27">
+        <f>H23+H25+H26</f>
         <v/>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="13" t="inlineStr">
-        <is>
-          <t>Total Equity</t>
-        </is>
-      </c>
-      <c r="B28" s="33">
-        <f>B26+B27</f>
-        <v/>
-      </c>
-      <c r="C28" s="33">
-        <f>C26+C27</f>
-        <v/>
-      </c>
-      <c r="D28" s="33">
-        <f>D26+D27</f>
-        <v/>
-      </c>
-      <c r="E28" s="33">
-        <f>E26+E27</f>
-        <v/>
-      </c>
-      <c r="F28" s="33">
-        <f>F26+F27</f>
-        <v/>
-      </c>
-      <c r="G28" s="33">
-        <f>G26+G27</f>
-        <v/>
-      </c>
-      <c r="H28" s="33">
-        <f>H26+H27</f>
-        <v/>
-      </c>
-      <c r="I28">
-        <f>I26+I27</f>
-        <v/>
-      </c>
+      <c r="A28" s="8" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="13" t="inlineStr">
         <is>
-          <t>Total Liab. + Equity</t>
-        </is>
-      </c>
-      <c r="B29" s="33">
-        <f>B23+B28</f>
-        <v/>
-      </c>
-      <c r="C29" s="33">
-        <f>C23+C28</f>
-        <v/>
-      </c>
-      <c r="D29" s="33">
-        <f>D23+D28</f>
-        <v/>
-      </c>
-      <c r="E29" s="33">
-        <f>E23+E28</f>
-        <v/>
-      </c>
-      <c r="F29" s="33">
-        <f>F23+F28</f>
-        <v/>
-      </c>
-      <c r="G29" s="33">
-        <f>G23+G28</f>
-        <v/>
-      </c>
-      <c r="H29" s="33">
-        <f>H23+H28</f>
-        <v/>
-      </c>
-      <c r="I29">
-        <f>I23+I28</f>
-        <v/>
+          <t>EQUITY</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8" t="inlineStr">
         <is>
+          <t>Retained Earnings</t>
+        </is>
+      </c>
+      <c r="B30" s="29">
+        <f>B16-B27-B31</f>
+        <v/>
+      </c>
+      <c r="C30" s="29">
+        <f>C16-C27-C31</f>
+        <v/>
+      </c>
+      <c r="D30" s="29">
+        <f>D16-D27-D31</f>
+        <v/>
+      </c>
+      <c r="E30" s="29">
+        <f>D30+'Income Statement'!E23</f>
+        <v/>
+      </c>
+      <c r="F30" s="29">
+        <f>E30+'Income Statement'!F23</f>
+        <v/>
+      </c>
+      <c r="G30" s="29">
+        <f>F30+'Income Statement'!G23</f>
+        <v/>
+      </c>
+      <c r="H30">
+        <f>G30+'Income Statement'!H23</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="inlineStr">
+        <is>
+          <t>Other Equity</t>
+        </is>
+      </c>
+      <c r="B31" s="14" t="n">
+        <v>20188</v>
+      </c>
+      <c r="C31" s="14" t="n">
+        <v>23321</v>
+      </c>
+      <c r="D31" s="14" t="n">
+        <v>28000</v>
+      </c>
+      <c r="E31" s="29">
+        <f>D31</f>
+        <v/>
+      </c>
+      <c r="F31" s="29">
+        <f>E31</f>
+        <v/>
+      </c>
+      <c r="G31" s="29">
+        <f>F31</f>
+        <v/>
+      </c>
+      <c r="H31">
+        <f>G31</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="13" t="inlineStr">
+        <is>
+          <t>Total Equity</t>
+        </is>
+      </c>
+      <c r="B32" s="33">
+        <f>B30+B31</f>
+        <v/>
+      </c>
+      <c r="C32" s="33">
+        <f>C30+C31</f>
+        <v/>
+      </c>
+      <c r="D32" s="33">
+        <f>D30+D31</f>
+        <v/>
+      </c>
+      <c r="E32" s="33">
+        <f>E30+E31</f>
+        <v/>
+      </c>
+      <c r="F32" s="33">
+        <f>F30+F31</f>
+        <v/>
+      </c>
+      <c r="G32" s="33">
+        <f>G30+G31</f>
+        <v/>
+      </c>
+      <c r="H32">
+        <f>H30+H31</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="13" t="inlineStr">
+        <is>
+          <t>Total Liab. + Equity</t>
+        </is>
+      </c>
+      <c r="B33" s="33">
+        <f>B27+B32</f>
+        <v/>
+      </c>
+      <c r="C33" s="33">
+        <f>C27+C32</f>
+        <v/>
+      </c>
+      <c r="D33" s="33">
+        <f>D27+D32</f>
+        <v/>
+      </c>
+      <c r="E33" s="33">
+        <f>E27+E32</f>
+        <v/>
+      </c>
+      <c r="F33" s="33">
+        <f>F27+F32</f>
+        <v/>
+      </c>
+      <c r="G33" s="33">
+        <f>G27+G32</f>
+        <v/>
+      </c>
+      <c r="H33">
+        <f>H27+H32</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="8" t="inlineStr">
+        <is>
           <t>Balance Check (should be 0)</t>
         </is>
       </c>
-      <c r="B30" s="29">
-        <f>B15-B29</f>
-        <v/>
-      </c>
-      <c r="C30" s="29">
-        <f>C15-C29</f>
-        <v/>
-      </c>
-      <c r="D30" s="29">
-        <f>D15-D29</f>
-        <v/>
-      </c>
-      <c r="E30" s="29">
-        <f>E15-E29</f>
-        <v/>
-      </c>
-      <c r="F30" s="29">
-        <f>F15-F29</f>
-        <v/>
-      </c>
-      <c r="G30" s="29">
-        <f>G15-G29</f>
-        <v/>
-      </c>
-      <c r="H30" s="29">
-        <f>H15-H29</f>
-        <v/>
-      </c>
-      <c r="I30" s="29">
-        <f>I15-I29</f>
+      <c r="B34" s="29">
+        <f>B16-B33</f>
+        <v/>
+      </c>
+      <c r="C34" s="29">
+        <f>C16-C33</f>
+        <v/>
+      </c>
+      <c r="D34" s="29">
+        <f>D16-D33</f>
+        <v/>
+      </c>
+      <c r="E34" s="29">
+        <f>E16-E33</f>
+        <v/>
+      </c>
+      <c r="F34" s="29">
+        <f>F16-F33</f>
+        <v/>
+      </c>
+      <c r="G34" s="29">
+        <f>G16-G33</f>
+        <v/>
+      </c>
+      <c r="H34" s="29">
+        <f>H16-H33</f>
         <v/>
       </c>
     </row>
@@ -2825,7 +2698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2841,13 +2714,12 @@
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="14" customWidth="1" min="7" max="7"/>
     <col width="14" customWidth="1" min="8" max="8"/>
-    <col width="14" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Cash Flow Statement — UBER ($M)</t>
+          <t>Cash Flow Statement � UBER ($M) [UPDATED POST Q4-2025]</t>
         </is>
       </c>
     </row>
@@ -2888,11 +2760,6 @@
           <t>2029E</t>
         </is>
       </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>2030E</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
@@ -2931,12 +2798,8 @@
         <f>'Income Statement'!G23</f>
         <v/>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="26">
         <f>'Income Statement'!H23</f>
-        <v/>
-      </c>
-      <c r="I5" s="26">
-        <f>'Income Statement'!I23</f>
         <v/>
       </c>
     </row>
@@ -2970,109 +2833,95 @@
         <f>'Income Statement'!G4*Assumptions!G9</f>
         <v/>
       </c>
-      <c r="H6" s="29">
+      <c r="H6">
         <f>'Income Statement'!H4*Assumptions!H9</f>
-        <v/>
-      </c>
-      <c r="I6">
-        <f>'Income Statement'!I4*Assumptions!I9</f>
         <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="8" t="inlineStr">
         <is>
-          <t>Changes in Working Capital</t>
-        </is>
-      </c>
-      <c r="B7" s="29" t="n"/>
-      <c r="C7" s="29" t="n"/>
-      <c r="D7" s="29" t="n"/>
-      <c r="E7" s="29">
-        <f>E8+E9+E10+E11</f>
-        <v/>
-      </c>
-      <c r="F7" s="29">
-        <f>F8+F9+F10+F11</f>
-        <v/>
-      </c>
-      <c r="G7" s="29">
-        <f>G8+G9+G10+G11</f>
-        <v/>
-      </c>
-      <c r="H7" s="29">
-        <f>H8+H9+H10+H11</f>
-        <v/>
-      </c>
-      <c r="I7">
-        <f>I8+I9+I10+I11</f>
-        <v/>
+          <t>Stock-Based Compensation</t>
+        </is>
+      </c>
+      <c r="B7" s="14" t="n">
+        <v>1900</v>
+      </c>
+      <c r="C7" s="14" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D7" s="14" t="n">
+        <v>1700</v>
+      </c>
+      <c r="E7" s="14" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F7" s="14" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G7" s="14" t="n">
+        <v>1500</v>
+      </c>
+      <c r="H7" s="28" t="n">
+        <v>1500</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Change in AR</t>
+          <t>Changes in Working Capital</t>
         </is>
       </c>
       <c r="B8" s="29" t="n"/>
       <c r="C8" s="29" t="n"/>
       <c r="D8" s="29" t="n"/>
       <c r="E8" s="29">
-        <f>-('Balance Sheet'!E7-'Balance Sheet'!D7)</f>
+        <f>E9+E10+E11+E12</f>
         <v/>
       </c>
       <c r="F8" s="29">
-        <f>-('Balance Sheet'!F7-'Balance Sheet'!E7)</f>
+        <f>F9+F10+F11+F12</f>
         <v/>
       </c>
       <c r="G8" s="29">
-        <f>-('Balance Sheet'!G7-'Balance Sheet'!F7)</f>
-        <v/>
-      </c>
-      <c r="H8" s="29">
-        <f>-('Balance Sheet'!H7-'Balance Sheet'!G7)</f>
-        <v/>
-      </c>
-      <c r="I8">
-        <f>-('Balance Sheet'!I7-'Balance Sheet'!H7)</f>
+        <f>G9+G10+G11+G12</f>
+        <v/>
+      </c>
+      <c r="H8">
+        <f>H9+H10+H11+H12</f>
         <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Change in AP</t>
+          <t xml:space="preserve">  Change in AR</t>
         </is>
       </c>
       <c r="B9" s="29" t="n"/>
       <c r="C9" s="29" t="n"/>
       <c r="D9" s="29" t="n"/>
       <c r="E9" s="29">
-        <f>'Balance Sheet'!E18-'Balance Sheet'!D18</f>
+        <f>-('Balance Sheet'!E7-'Balance Sheet'!D7)</f>
         <v/>
       </c>
       <c r="F9" s="29">
-        <f>'Balance Sheet'!F18-'Balance Sheet'!E18</f>
+        <f>-('Balance Sheet'!F7-'Balance Sheet'!E7)</f>
         <v/>
       </c>
       <c r="G9" s="29">
-        <f>'Balance Sheet'!G18-'Balance Sheet'!F18</f>
-        <v/>
-      </c>
-      <c r="H9" s="29">
-        <f>'Balance Sheet'!H18-'Balance Sheet'!G18</f>
-        <v/>
-      </c>
-      <c r="I9">
-        <f>'Balance Sheet'!I18-'Balance Sheet'!H18</f>
+        <f>-('Balance Sheet'!G7-'Balance Sheet'!F7)</f>
+        <v/>
+      </c>
+      <c r="H9">
+        <f>-('Balance Sheet'!H7-'Balance Sheet'!G7)</f>
         <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Change in Accrued Liab</t>
+          <t xml:space="preserve">  Change in AP</t>
         </is>
       </c>
       <c r="B10" s="29" t="n"/>
@@ -3090,194 +2939,195 @@
         <f>'Balance Sheet'!G19-'Balance Sheet'!F19</f>
         <v/>
       </c>
-      <c r="H10" s="29">
+      <c r="H10">
         <f>'Balance Sheet'!H19-'Balance Sheet'!G19</f>
-        <v/>
-      </c>
-      <c r="I10">
-        <f>'Balance Sheet'!I19-'Balance Sheet'!H19</f>
         <v/>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Other Operating Changes</t>
+          <t xml:space="preserve">  Change in Accrued Liab</t>
         </is>
       </c>
       <c r="B11" s="29" t="n"/>
       <c r="C11" s="29" t="n"/>
       <c r="D11" s="29" t="n"/>
-      <c r="E11" s="14" t="n">
+      <c r="E11" s="29">
+        <f>'Balance Sheet'!E20-'Balance Sheet'!D20</f>
+        <v/>
+      </c>
+      <c r="F11" s="29">
+        <f>'Balance Sheet'!F20-'Balance Sheet'!E20</f>
+        <v/>
+      </c>
+      <c r="G11" s="29">
+        <f>'Balance Sheet'!G20-'Balance Sheet'!F20</f>
+        <v/>
+      </c>
+      <c r="H11">
+        <f>'Balance Sheet'!H20-'Balance Sheet'!G20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Other Operating Changes</t>
+        </is>
+      </c>
+      <c r="B12" s="29" t="n"/>
+      <c r="C12" s="29" t="n"/>
+      <c r="D12" s="29" t="n"/>
+      <c r="E12" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="14" t="n">
+      <c r="F12" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="14" t="n">
+      <c r="G12" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="H11" s="14" t="n">
+      <c r="H12" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="28" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="13" t="inlineStr">
+    </row>
+    <row r="13">
+      <c r="A13" s="13" t="inlineStr">
         <is>
           <t>Cash from Operations (CFO)</t>
         </is>
       </c>
-      <c r="B12" s="33" t="n">
-        <v>3585</v>
-      </c>
-      <c r="C12" s="33" t="n">
-        <v>6903</v>
-      </c>
-      <c r="D12" s="33" t="n">
-        <v>9760</v>
-      </c>
-      <c r="E12" s="33">
-        <f>E5+E6+E7</f>
-        <v/>
-      </c>
-      <c r="F12" s="33">
-        <f>F5+F6+F7</f>
-        <v/>
-      </c>
-      <c r="G12" s="33">
-        <f>G5+G6+G7</f>
-        <v/>
-      </c>
-      <c r="H12" s="33">
-        <f>H5+H6+H7</f>
-        <v/>
-      </c>
-      <c r="I12">
-        <f>I5+I6+I7</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="8" t="inlineStr"/>
+      <c r="B13" s="33" t="n">
+        <v>6867</v>
+      </c>
+      <c r="C13" s="33" t="n">
+        <v>7490</v>
+      </c>
+      <c r="D13" s="33" t="n">
+        <v>10100</v>
+      </c>
+      <c r="E13" s="33">
+        <f>E5+E6+E7+E8</f>
+        <v/>
+      </c>
+      <c r="F13" s="33">
+        <f>F5+F6+F7+F8</f>
+        <v/>
+      </c>
+      <c r="G13" s="33">
+        <f>G5+G6+G7+G8</f>
+        <v/>
+      </c>
+      <c r="H13">
+        <f>H5+H6+H7+H8</f>
+        <v/>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="13" t="inlineStr">
+      <c r="A14" s="8" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="13" t="inlineStr">
         <is>
           <t>INVESTING ACTIVITIES</t>
         </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="8" t="inlineStr">
-        <is>
-          <t>(-) Capital Expenditures</t>
-        </is>
-      </c>
-      <c r="B15" s="14" t="n">
-        <v>600</v>
-      </c>
-      <c r="C15" s="14" t="n">
-        <v>650</v>
-      </c>
-      <c r="D15" s="14" t="n">
-        <v>700</v>
-      </c>
-      <c r="E15" s="29">
-        <f>'Income Statement'!E4*Assumptions!E12</f>
-        <v/>
-      </c>
-      <c r="F15" s="29">
-        <f>'Income Statement'!F4*Assumptions!F12</f>
-        <v/>
-      </c>
-      <c r="G15" s="29">
-        <f>'Income Statement'!G4*Assumptions!G12</f>
-        <v/>
-      </c>
-      <c r="H15" s="29">
-        <f>'Income Statement'!H4*Assumptions!H12</f>
-        <v/>
-      </c>
-      <c r="I15">
-        <f>'Income Statement'!I4*Assumptions!I12</f>
-        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8" t="inlineStr">
         <is>
-          <t>(-) Other Investing</t>
+          <t>(-) Capital Expenditures</t>
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>-500</v>
+        <v>620</v>
       </c>
       <c r="C16" s="14" t="n">
-        <v>-500</v>
+        <v>750</v>
       </c>
       <c r="D16" s="14" t="n">
-        <v>-500</v>
-      </c>
-      <c r="E16" s="14" t="n">
-        <v>-300</v>
-      </c>
-      <c r="F16" s="14" t="n">
-        <v>-300</v>
-      </c>
-      <c r="G16" s="14" t="n">
-        <v>-300</v>
-      </c>
-      <c r="H16" s="14" t="n">
-        <v>-300</v>
-      </c>
-      <c r="I16" s="28" t="n">
-        <v>-300</v>
+        <v>900</v>
+      </c>
+      <c r="E16" s="29">
+        <f>'Income Statement'!E4*Assumptions!E12</f>
+        <v/>
+      </c>
+      <c r="F16" s="29">
+        <f>'Income Statement'!F4*Assumptions!F12</f>
+        <v/>
+      </c>
+      <c r="G16" s="29">
+        <f>'Income Statement'!G4*Assumptions!G12</f>
+        <v/>
+      </c>
+      <c r="H16">
+        <f>'Income Statement'!H4*Assumptions!H12</f>
+        <v/>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="13" t="inlineStr">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>(-) Net Investment Changes</t>
+        </is>
+      </c>
+      <c r="B17" s="14" t="n">
+        <v>-200</v>
+      </c>
+      <c r="C17" s="14" t="n">
+        <v>-200</v>
+      </c>
+      <c r="D17" s="14" t="n">
+        <v>-200</v>
+      </c>
+      <c r="E17" s="14" t="n">
+        <v>-200</v>
+      </c>
+      <c r="F17" s="14" t="n">
+        <v>-200</v>
+      </c>
+      <c r="G17" s="14" t="n">
+        <v>-200</v>
+      </c>
+      <c r="H17" s="28" t="n">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="13" t="inlineStr">
         <is>
           <t>Cash from Investing (CFI)</t>
         </is>
       </c>
-      <c r="B17" s="33">
-        <f>-B15+B16</f>
-        <v/>
-      </c>
-      <c r="C17" s="33">
-        <f>-C15+C16</f>
-        <v/>
-      </c>
-      <c r="D17" s="33">
-        <f>-D15+D16</f>
-        <v/>
-      </c>
-      <c r="E17" s="33">
-        <f>-E15+E16</f>
-        <v/>
-      </c>
-      <c r="F17" s="33">
-        <f>-F15+F16</f>
-        <v/>
-      </c>
-      <c r="G17" s="33">
-        <f>-G15+G16</f>
-        <v/>
-      </c>
-      <c r="H17" s="33">
-        <f>-H15+H16</f>
-        <v/>
-      </c>
-      <c r="I17">
-        <f>-I15+I16</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="8" t="inlineStr"/>
+      <c r="B18" s="33">
+        <f>-B16+B17</f>
+        <v/>
+      </c>
+      <c r="C18" s="33">
+        <f>-C16+C17</f>
+        <v/>
+      </c>
+      <c r="D18" s="33">
+        <f>-D16+D17</f>
+        <v/>
+      </c>
+      <c r="E18" s="33">
+        <f>-E16+E17</f>
+        <v/>
+      </c>
+      <c r="F18" s="33">
+        <f>-F16+F17</f>
+        <v/>
+      </c>
+      <c r="G18" s="33">
+        <f>-G16+G17</f>
+        <v/>
+      </c>
+      <c r="H18">
+        <f>-H16+H17</f>
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="13" t="inlineStr">
@@ -3286,35 +3136,31 @@
         </is>
       </c>
       <c r="B19" s="33">
-        <f>B12+B17</f>
+        <f>B13+B18</f>
         <v/>
       </c>
       <c r="C19" s="33">
-        <f>C12+C17</f>
+        <f>C13+C18</f>
         <v/>
       </c>
       <c r="D19" s="33">
-        <f>D12+D17</f>
+        <f>D13+D18</f>
         <v/>
       </c>
       <c r="E19" s="33">
-        <f>E12+E17</f>
+        <f>E13+E18</f>
         <v/>
       </c>
       <c r="F19" s="33">
-        <f>F12+F17</f>
+        <f>F13+F18</f>
         <v/>
       </c>
       <c r="G19" s="33">
-        <f>G12+G17</f>
-        <v/>
-      </c>
-      <c r="H19" s="33">
-        <f>H12+H17</f>
-        <v/>
-      </c>
-      <c r="I19">
-        <f>I12+I17</f>
+        <f>G13+G18</f>
+        <v/>
+      </c>
+      <c r="H19">
+        <f>H13+H18</f>
         <v/>
       </c>
     </row>

</xml_diff>